<commit_message>
working on GP non0-linear
</commit_message>
<xml_diff>
--- a/results/forAvi/distSmry_results.xlsx
+++ b/results/forAvi/distSmry_results.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex Palomino\Documents\GitHub\EV-Flexibility\results\forAvi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF758311-4427-4DB4-A9EC-5D3682069CFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A733B4-BF28-40C0-A330-B61A6BB2EE3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WorkplaceSmry" sheetId="1" r:id="rId1"/>
-    <sheet name="PublicSmry" sheetId="2" r:id="rId2"/>
+    <sheet name="WorkplaceProb" sheetId="4" r:id="rId2"/>
+    <sheet name="PublicSmry" sheetId="2" r:id="rId3"/>
+    <sheet name="PublicProb" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="35">
   <si>
     <t>mean</t>
   </si>
@@ -125,6 +127,12 @@
   </si>
   <si>
     <t>mu__23</t>
+  </si>
+  <si>
+    <t>Hr</t>
+  </si>
+  <si>
+    <t>EV Count</t>
   </si>
 </sst>
 </file>
@@ -1168,10 +1176,1367 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09BC618A-F583-4917-B0F1-3C5C1ABDF366}">
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2">
+        <v>9</v>
+      </c>
+      <c r="L2" s="2">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2">
+        <v>12</v>
+      </c>
+      <c r="O2" s="2">
+        <v>13</v>
+      </c>
+      <c r="P2" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="C3">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D3">
+        <v>1E-3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.97760000000000002</v>
+      </c>
+      <c r="C4">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="D4">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="C5">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0.99919999999999998</v>
+      </c>
+      <c r="C6">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0.9798</v>
+      </c>
+      <c r="C7">
+        <v>0.02</v>
+      </c>
+      <c r="D7">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="C8">
+        <v>0.184</v>
+      </c>
+      <c r="D8">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>2.8E-3</v>
+      </c>
+      <c r="F8">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>0.15939999999999999</v>
+      </c>
+      <c r="C9">
+        <v>0.29859999999999998</v>
+      </c>
+      <c r="D9">
+        <v>0.25879999999999997</v>
+      </c>
+      <c r="E9">
+        <v>0.16439999999999999</v>
+      </c>
+      <c r="F9">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.03</v>
+      </c>
+      <c r="H9">
+        <v>7.6E-3</v>
+      </c>
+      <c r="I9">
+        <v>1.4E-3</v>
+      </c>
+      <c r="J9">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="K9">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>4.1200000000000001E-2</v>
+      </c>
+      <c r="C10">
+        <v>0.1308</v>
+      </c>
+      <c r="D10">
+        <v>0.21360000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.21179999999999999</v>
+      </c>
+      <c r="F10">
+        <v>0.17560000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.1236</v>
+      </c>
+      <c r="H10">
+        <v>6.1199999999999997E-2</v>
+      </c>
+      <c r="I10">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="J10">
+        <v>1.04E-2</v>
+      </c>
+      <c r="K10">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="L10">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="M10">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="N10">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.20119999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.3196</v>
+      </c>
+      <c r="D11">
+        <v>0.25440000000000002</v>
+      </c>
+      <c r="E11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F11">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G11">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="H11">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="I11">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J11">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0.54039999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.33760000000000001</v>
+      </c>
+      <c r="D12">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="E12">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="F12">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.39939999999999998</v>
+      </c>
+      <c r="C13">
+        <v>0.3644</v>
+      </c>
+      <c r="D13">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E13">
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="F13">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="G13">
+        <v>2E-3</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>0.24479999999999999</v>
+      </c>
+      <c r="C14">
+        <v>0.3518</v>
+      </c>
+      <c r="D14">
+        <v>0.24179999999999999</v>
+      </c>
+      <c r="E14">
+        <v>0.1142</v>
+      </c>
+      <c r="F14">
+        <v>3.3799999999999997E-2</v>
+      </c>
+      <c r="G14">
+        <v>1.04E-2</v>
+      </c>
+      <c r="H14">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="I14">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="J14">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="C15">
+        <v>0.1938</v>
+      </c>
+      <c r="D15">
+        <v>0.25619999999999998</v>
+      </c>
+      <c r="E15">
+        <v>0.21379999999999999</v>
+      </c>
+      <c r="F15">
+        <v>0.13819999999999999</v>
+      </c>
+      <c r="G15">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="H15">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="I15">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="J15">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="K15">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="L15">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="M15">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>9.6600000000000005E-2</v>
+      </c>
+      <c r="C16">
+        <v>0.22919999999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.25819999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.2092</v>
+      </c>
+      <c r="F16">
+        <v>0.1212</v>
+      </c>
+      <c r="G16">
+        <v>5.62E-2</v>
+      </c>
+      <c r="H16">
+        <v>1.9E-2</v>
+      </c>
+      <c r="I16">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="J16">
+        <v>1.8E-3</v>
+      </c>
+      <c r="K16">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>0.188</v>
+      </c>
+      <c r="C17">
+        <v>0.31559999999999999</v>
+      </c>
+      <c r="D17">
+        <v>0.26719999999999999</v>
+      </c>
+      <c r="E17">
+        <v>0.14119999999999999</v>
+      </c>
+      <c r="F17">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="G17">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="H17">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="I17">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J17">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="K17">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="C18">
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.27079999999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.18379999999999999</v>
+      </c>
+      <c r="F18">
+        <v>9.8400000000000001E-2</v>
+      </c>
+      <c r="G18">
+        <v>3.3799999999999997E-2</v>
+      </c>
+      <c r="H18">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="I18">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="J18">
+        <v>1E-3</v>
+      </c>
+      <c r="K18">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>0.46560000000000001</v>
+      </c>
+      <c r="C19">
+        <v>0.36659999999999998</v>
+      </c>
+      <c r="D19">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="E19">
+        <v>2.7400000000000001E-2</v>
+      </c>
+      <c r="F19">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="G19">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="H19">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="C20">
+        <v>0.1948</v>
+      </c>
+      <c r="D20">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E20">
+        <v>1E-3</v>
+      </c>
+      <c r="F20">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>0.751</v>
+      </c>
+      <c r="C21">
+        <v>0.2094</v>
+      </c>
+      <c r="D21">
+        <v>3.6200000000000003E-2</v>
+      </c>
+      <c r="E21">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F21">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>0.84060000000000001</v>
+      </c>
+      <c r="C22">
+        <v>0.1454</v>
+      </c>
+      <c r="D22">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="E22">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>0.74839999999999995</v>
+      </c>
+      <c r="C23">
+        <v>0.2218</v>
+      </c>
+      <c r="D23">
+        <v>2.64E-2</v>
+      </c>
+      <c r="E23">
+        <v>3.3999999999999998E-3</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>0.80220000000000002</v>
+      </c>
+      <c r="C24">
+        <v>0.18179999999999999</v>
+      </c>
+      <c r="D24">
+        <v>1.44E-2</v>
+      </c>
+      <c r="E24">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>0.4506</v>
+      </c>
+      <c r="C25">
+        <v>0.36159999999999998</v>
+      </c>
+      <c r="D25">
+        <v>0.1414</v>
+      </c>
+      <c r="E25">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="F25">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="G25">
+        <v>2E-3</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="C26">
+        <v>0.371</v>
+      </c>
+      <c r="D26">
+        <v>0.15820000000000001</v>
+      </c>
+      <c r="E26">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="F26">
+        <v>1.04E-2</v>
+      </c>
+      <c r="G26">
+        <v>1.4E-3</v>
+      </c>
+      <c r="H26">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:Q26">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0256CB3-F23A-40D4-9C7A-5791A12E21BE}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -1880,4 +3245,1362 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E345E-C114-47BB-881B-1817599095D4}">
+  <dimension ref="A1:Q26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2">
+        <v>9</v>
+      </c>
+      <c r="L2" s="2">
+        <v>10</v>
+      </c>
+      <c r="M2" s="2">
+        <v>11</v>
+      </c>
+      <c r="N2" s="2">
+        <v>12</v>
+      </c>
+      <c r="O2" s="2">
+        <v>13</v>
+      </c>
+      <c r="P2" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0.94</v>
+      </c>
+      <c r="C3">
+        <v>5.74E-2</v>
+      </c>
+      <c r="D3">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="C4">
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="D4">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.98860000000000003</v>
+      </c>
+      <c r="C5">
+        <v>1.14E-2</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0.99380000000000002</v>
+      </c>
+      <c r="C6">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0.99519999999999997</v>
+      </c>
+      <c r="C7">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="C8">
+        <v>0.31159999999999999</v>
+      </c>
+      <c r="D8">
+        <v>9.0200000000000002E-2</v>
+      </c>
+      <c r="E8">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="F8">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>0.30480000000000002</v>
+      </c>
+      <c r="C9">
+        <v>0.37459999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.2054</v>
+      </c>
+      <c r="E9">
+        <v>8.4199999999999997E-2</v>
+      </c>
+      <c r="F9">
+        <v>2.4199999999999999E-2</v>
+      </c>
+      <c r="G9">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="H9">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>0.23619999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.3352</v>
+      </c>
+      <c r="D10">
+        <v>0.251</v>
+      </c>
+      <c r="E10">
+        <v>0.122</v>
+      </c>
+      <c r="F10">
+        <v>3.8800000000000001E-2</v>
+      </c>
+      <c r="G10">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="H10">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I10">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="J10">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="C11">
+        <v>0.08</v>
+      </c>
+      <c r="D11">
+        <v>0.15840000000000001</v>
+      </c>
+      <c r="E11">
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.192</v>
+      </c>
+      <c r="G11">
+        <v>0.15060000000000001</v>
+      </c>
+      <c r="H11">
+        <v>9.8199999999999996E-2</v>
+      </c>
+      <c r="I11">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="J11">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="K11">
+        <v>1.24E-2</v>
+      </c>
+      <c r="L11">
+        <v>3.8E-3</v>
+      </c>
+      <c r="M11">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="N11">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.1628</v>
+      </c>
+      <c r="D12">
+        <v>0.22259999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.22420000000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.17180000000000001</v>
+      </c>
+      <c r="G12">
+        <v>0.09</v>
+      </c>
+      <c r="H12">
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="I12">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="J12">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="K12">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="L12">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="C13">
+        <v>0.189</v>
+      </c>
+      <c r="D13">
+        <v>0.2472</v>
+      </c>
+      <c r="E13">
+        <v>0.21579999999999999</v>
+      </c>
+      <c r="F13">
+        <v>0.14680000000000001</v>
+      </c>
+      <c r="G13">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="H13">
+        <v>2.86E-2</v>
+      </c>
+      <c r="I13">
+        <v>1.32E-2</v>
+      </c>
+      <c r="J13">
+        <v>3.8E-3</v>
+      </c>
+      <c r="K13">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="L13">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="C14">
+        <v>0.18859999999999999</v>
+      </c>
+      <c r="D14">
+        <v>0.25</v>
+      </c>
+      <c r="E14">
+        <v>0.21460000000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G14">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="H14">
+        <v>3.56E-2</v>
+      </c>
+      <c r="I14">
+        <v>1.38E-2</v>
+      </c>
+      <c r="J14">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="K14">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="L14">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="C15">
+        <v>0.1842</v>
+      </c>
+      <c r="D15">
+        <v>0.2344</v>
+      </c>
+      <c r="E15">
+        <v>0.22520000000000001</v>
+      </c>
+      <c r="F15">
+        <v>0.15640000000000001</v>
+      </c>
+      <c r="G15">
+        <v>8.1799999999999998E-2</v>
+      </c>
+      <c r="H15">
+        <v>3.9199999999999999E-2</v>
+      </c>
+      <c r="I15">
+        <v>1.18E-2</v>
+      </c>
+      <c r="J15">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="K15">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="L15">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="M15">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="N15">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>7.7600000000000002E-2</v>
+      </c>
+      <c r="C16">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.24479999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.21759999999999999</v>
+      </c>
+      <c r="F16">
+        <v>0.1492</v>
+      </c>
+      <c r="G16">
+        <v>8.2600000000000007E-2</v>
+      </c>
+      <c r="H16">
+        <v>3.5799999999999998E-2</v>
+      </c>
+      <c r="I16">
+        <v>1.46E-2</v>
+      </c>
+      <c r="J16">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="K16">
+        <v>1.4E-3</v>
+      </c>
+      <c r="L16">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>8.0399999999999999E-2</v>
+      </c>
+      <c r="C17">
+        <v>0.18679999999999999</v>
+      </c>
+      <c r="D17">
+        <v>0.24979999999999999</v>
+      </c>
+      <c r="E17">
+        <v>0.2278</v>
+      </c>
+      <c r="F17">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="G17">
+        <v>7.2800000000000004E-2</v>
+      </c>
+      <c r="H17">
+        <v>2.98E-2</v>
+      </c>
+      <c r="I17">
+        <v>1.04E-2</v>
+      </c>
+      <c r="J17">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="K17">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="L17">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>0.11459999999999999</v>
+      </c>
+      <c r="C18">
+        <v>0.2424</v>
+      </c>
+      <c r="D18">
+        <v>0.2676</v>
+      </c>
+      <c r="E18">
+        <v>0.1976</v>
+      </c>
+      <c r="F18">
+        <v>0.10340000000000001</v>
+      </c>
+      <c r="G18">
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="H18">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="I18">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="J18">
+        <v>1.4E-3</v>
+      </c>
+      <c r="K18">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" s="2">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>0.1004</v>
+      </c>
+      <c r="C19">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D19">
+        <v>0.25879999999999997</v>
+      </c>
+      <c r="E19">
+        <v>0.2036</v>
+      </c>
+      <c r="F19">
+        <v>0.1192</v>
+      </c>
+      <c r="G19">
+        <v>5.5599999999999997E-2</v>
+      </c>
+      <c r="H19">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="I19">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="J19">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="K19">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="L19">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="C20">
+        <v>0.16120000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.24579999999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.22159999999999999</v>
+      </c>
+      <c r="F20">
+        <v>0.15040000000000001</v>
+      </c>
+      <c r="G20">
+        <v>9.1600000000000001E-2</v>
+      </c>
+      <c r="H20">
+        <v>3.9E-2</v>
+      </c>
+      <c r="I20">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="J20">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="K20">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="L20">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M20">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="N20">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>4.7199999999999999E-2</v>
+      </c>
+      <c r="C21">
+        <v>0.14660000000000001</v>
+      </c>
+      <c r="D21">
+        <v>0.21740000000000001</v>
+      </c>
+      <c r="E21">
+        <v>0.22140000000000001</v>
+      </c>
+      <c r="F21">
+        <v>0.17560000000000001</v>
+      </c>
+      <c r="G21">
+        <v>0.1</v>
+      </c>
+      <c r="H21">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="I21">
+        <v>2.64E-2</v>
+      </c>
+      <c r="J21">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="K21">
+        <v>2.8E-3</v>
+      </c>
+      <c r="L21">
+        <v>1E-3</v>
+      </c>
+      <c r="M21">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>0.13739999999999999</v>
+      </c>
+      <c r="C22">
+        <v>0.27479999999999999</v>
+      </c>
+      <c r="D22">
+        <v>0.2666</v>
+      </c>
+      <c r="E22">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="F22">
+        <v>9.06E-2</v>
+      </c>
+      <c r="G22">
+        <v>3.6600000000000001E-2</v>
+      </c>
+      <c r="H22">
+        <v>1.34E-2</v>
+      </c>
+      <c r="I22">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="J22">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="K22">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>0.38619999999999999</v>
+      </c>
+      <c r="C23">
+        <v>0.35420000000000001</v>
+      </c>
+      <c r="D23">
+        <v>0.185</v>
+      </c>
+      <c r="E23">
+        <v>5.8400000000000001E-2</v>
+      </c>
+      <c r="F23">
+        <v>1.34E-2</v>
+      </c>
+      <c r="G23">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="H23">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="I23">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" s="2">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>0.5736</v>
+      </c>
+      <c r="C24">
+        <v>0.31859999999999999</v>
+      </c>
+      <c r="D24">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="E24">
+        <v>1.72E-2</v>
+      </c>
+      <c r="F24">
+        <v>2.8E-3</v>
+      </c>
+      <c r="G24">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" s="2">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>0.69940000000000002</v>
+      </c>
+      <c r="C25">
+        <v>0.25</v>
+      </c>
+      <c r="D25">
+        <v>4.1599999999999998E-2</v>
+      </c>
+      <c r="E25">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F25">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="G25">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A26" s="2">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>0.87360000000000004</v>
+      </c>
+      <c r="C26">
+        <v>0.1162</v>
+      </c>
+      <c r="D26">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="E26">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B3:Q26">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>